<commit_message>
Comp 230 functionality completed
</commit_message>
<xml_diff>
--- a/src/python/Comp230/invoice_template.xlsx
+++ b/src/python/Comp230/invoice_template.xlsx
@@ -9,7 +9,7 @@
     <sheet name="Invoice Template" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -835,7 +835,16 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -845,25 +854,33 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="23" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,23 +895,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1303,24 +1303,24 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="3.42578125" customWidth="1" style="62" min="1" max="1"/>
-    <col width="25.85546875" customWidth="1" style="62" min="2" max="2"/>
-    <col width="4.5703125" customWidth="1" style="62" min="3" max="3"/>
-    <col width="36.85546875" customWidth="1" style="62" min="4" max="4"/>
-    <col width="7.42578125" customWidth="1" style="62" min="5" max="5"/>
-    <col width="16.42578125" customWidth="1" style="62" min="6" max="6"/>
-    <col width="14.7109375" customWidth="1" style="62" min="7" max="7"/>
-    <col width="16.85546875" customWidth="1" style="62" min="8" max="8"/>
-    <col width="4" customWidth="1" style="62" min="9" max="9"/>
+    <col width="3.42578125" customWidth="1" style="60" min="1" max="1"/>
+    <col width="25.85546875" customWidth="1" style="60" min="2" max="2"/>
+    <col width="4.5703125" customWidth="1" style="60" min="3" max="3"/>
+    <col width="36.85546875" customWidth="1" style="60" min="4" max="4"/>
+    <col width="7.42578125" customWidth="1" style="60" min="5" max="5"/>
+    <col width="16.42578125" customWidth="1" style="60" min="6" max="6"/>
+    <col width="14.7109375" customWidth="1" style="60" min="7" max="7"/>
+    <col width="16.85546875" customWidth="1" style="60" min="8" max="8"/>
+    <col width="4" customWidth="1" style="60" min="9" max="9"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1" s="62">
+    <row r="1" ht="14.25" customHeight="1" s="60">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="n"/>
       <c r="C1" s="2" t="n"/>
@@ -1331,7 +1331,7 @@
       <c r="H1" s="5" t="n"/>
       <c r="I1" s="5" t="n"/>
     </row>
-    <row r="2" ht="14.25" customHeight="1" s="62">
+    <row r="2" ht="14.25" customHeight="1" s="60">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="2" t="n"/>
@@ -1342,7 +1342,7 @@
       <c r="H2" s="5" t="n"/>
       <c r="I2" s="5" t="n"/>
     </row>
-    <row r="3" ht="76.5" customHeight="1" s="62">
+    <row r="3" ht="76.5" customHeight="1" s="60">
       <c r="A3" s="6" t="n"/>
       <c r="B3" s="6" t="inlineStr">
         <is>
@@ -1357,9 +1357,9 @@
       <c r="H3" s="9" t="n"/>
       <c r="I3" s="10" t="n"/>
     </row>
-    <row r="4" ht="18" customHeight="1" s="62">
+    <row r="4" ht="18" customHeight="1" s="60">
       <c r="A4" s="11" t="n"/>
-      <c r="B4" s="70" t="n"/>
+      <c r="B4" s="61" t="n"/>
       <c r="C4" s="8" t="n"/>
       <c r="D4" s="8" t="n"/>
       <c r="E4" s="2" t="n"/>
@@ -1371,12 +1371,12 @@
       </c>
       <c r="H4" s="13" t="inlineStr">
         <is>
-          <t>03-31-19</t>
+          <t>04-28-19</t>
         </is>
       </c>
       <c r="I4" s="14" t="n"/>
     </row>
-    <row r="5" ht="18" customHeight="1" s="62">
+    <row r="5" ht="18" customHeight="1" s="60">
       <c r="A5" s="11" t="n"/>
       <c r="C5" s="8" t="n"/>
       <c r="D5" s="8" t="n"/>
@@ -1386,7 +1386,7 @@
       <c r="H5" s="16" t="n"/>
       <c r="I5" s="16" t="n"/>
     </row>
-    <row r="6" ht="18" customHeight="1" s="62">
+    <row r="6" ht="18" customHeight="1" s="60">
       <c r="A6" s="11" t="n"/>
       <c r="C6" s="8" t="n"/>
       <c r="D6" s="8" t="n"/>
@@ -1398,21 +1398,21 @@
         </is>
       </c>
       <c r="H6" s="76" t="n">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="I6" s="14" t="n"/>
     </row>
-    <row r="7" ht="18" customHeight="1" s="62">
+    <row r="7" ht="18" customHeight="1" s="60">
       <c r="A7" s="11" t="n"/>
       <c r="C7" s="8" t="n"/>
       <c r="D7" s="8" t="n"/>
       <c r="E7" s="2" t="n"/>
-      <c r="F7" s="71" t="n"/>
+      <c r="F7" s="64" t="n"/>
       <c r="G7" s="2" t="n"/>
-      <c r="H7" s="71" t="n"/>
-      <c r="I7" s="71" t="n"/>
-    </row>
-    <row r="8" ht="18" customHeight="1" s="62">
+      <c r="H7" s="64" t="n"/>
+      <c r="I7" s="64" t="n"/>
+    </row>
+    <row r="8" ht="18" customHeight="1" s="60">
       <c r="A8" s="11" t="n"/>
       <c r="C8" s="8" t="n"/>
       <c r="D8" s="8" t="n"/>
@@ -1424,23 +1424,23 @@
         </is>
       </c>
       <c r="H8" s="76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I8" s="12" t="n"/>
     </row>
-    <row r="9" ht="18" customHeight="1" s="62">
+    <row r="9" ht="18" customHeight="1" s="60">
       <c r="A9" s="18" t="n"/>
       <c r="C9" s="8" t="n"/>
       <c r="D9" s="19" t="n"/>
       <c r="E9" s="2" t="n"/>
-      <c r="F9" s="69" t="inlineStr">
+      <c r="F9" s="59" t="inlineStr">
         <is>
           <t>&lt;Payment terms (due on receipt)&gt;</t>
         </is>
       </c>
-      <c r="I9" s="69" t="n"/>
-    </row>
-    <row r="10" ht="15.75" customHeight="1" s="62">
+      <c r="I9" s="59" t="n"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" s="60">
       <c r="A10" s="18" t="n"/>
       <c r="B10" s="18" t="n"/>
       <c r="C10" s="8" t="n"/>
@@ -1459,7 +1459,7 @@
       <c r="H10" s="21" t="n"/>
       <c r="I10" s="22" t="n"/>
     </row>
-    <row r="11" ht="4.5" customHeight="1" s="62">
+    <row r="11" ht="4.5" customHeight="1" s="60">
       <c r="A11" s="18" t="n"/>
       <c r="B11" s="18" t="n"/>
       <c r="C11" s="8" t="n"/>
@@ -1470,7 +1470,7 @@
       <c r="H11" s="2" t="n"/>
       <c r="I11" s="2" t="n"/>
     </row>
-    <row r="12" ht="18" customHeight="1" s="62">
+    <row r="12" ht="18" customHeight="1" s="60">
       <c r="A12" s="18" t="n"/>
       <c r="B12" s="23" t="inlineStr">
         <is>
@@ -1480,20 +1480,20 @@
       <c r="C12" s="8" t="n"/>
       <c r="D12" s="25" t="inlineStr">
         <is>
-          <t>Baker Holder</t>
+          <t>Lila Odom</t>
         </is>
       </c>
       <c r="E12" s="24" t="n"/>
       <c r="F12" s="25" t="inlineStr">
         <is>
-          <t>Baker Holder</t>
+          <t>Lila Odom</t>
         </is>
       </c>
       <c r="G12" s="25" t="n"/>
       <c r="H12" s="25" t="n"/>
       <c r="I12" s="25" t="n"/>
     </row>
-    <row r="13" ht="18" customHeight="1" s="62">
+    <row r="13" ht="18" customHeight="1" s="60">
       <c r="A13" s="18" t="n"/>
       <c r="B13" s="23" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
       <c r="H13" s="25" t="n"/>
       <c r="I13" s="25" t="n"/>
     </row>
-    <row r="14" ht="18" customHeight="1" s="62">
+    <row r="14" ht="18" customHeight="1" s="60">
       <c r="A14" s="18" t="n"/>
       <c r="B14" s="23" t="inlineStr">
         <is>
@@ -1518,20 +1518,20 @@
       <c r="C14" s="8" t="n"/>
       <c r="D14" s="25" t="inlineStr">
         <is>
-          <t>P.O. Box 713, 8524 Metus. Av.</t>
+          <t>825-3804 Vitae, Rd.</t>
         </is>
       </c>
       <c r="E14" s="24" t="n"/>
       <c r="F14" s="25" t="inlineStr">
         <is>
-          <t>P.O. Box 713, 8524 Metus. Av.</t>
+          <t>825-3804 Vitae, Rd.</t>
         </is>
       </c>
       <c r="G14" s="25" t="n"/>
       <c r="H14" s="25" t="n"/>
       <c r="I14" s="25" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="62">
+    <row r="15" ht="18" customHeight="1" s="60">
       <c r="A15" s="18" t="n"/>
       <c r="B15" s="23" t="inlineStr">
         <is>
@@ -1541,20 +1541,20 @@
       <c r="C15" s="8" t="n"/>
       <c r="D15" s="25" t="inlineStr">
         <is>
-          <t>1-497-484-0330</t>
+          <t>1-752-766-5904</t>
         </is>
       </c>
       <c r="E15" s="24" t="n"/>
       <c r="F15" s="25" t="inlineStr">
         <is>
-          <t>1-497-484-0330</t>
+          <t>1-752-766-5904</t>
         </is>
       </c>
       <c r="G15" s="25" t="n"/>
       <c r="H15" s="25" t="n"/>
       <c r="I15" s="25" t="n"/>
     </row>
-    <row r="16" ht="18" customHeight="1" s="62">
+    <row r="16" ht="18" customHeight="1" s="60">
       <c r="A16" s="18" t="n"/>
       <c r="B16" s="23" t="inlineStr">
         <is>
@@ -1564,7 +1564,7 @@
       <c r="C16" s="8" t="n"/>
       <c r="D16" s="25" t="inlineStr">
         <is>
-          <t>bholder@fermentumfermentum.co.uk</t>
+          <t>lilia.odom@in.ca</t>
         </is>
       </c>
       <c r="E16" s="24" t="n"/>
@@ -1573,7 +1573,7 @@
       <c r="H16" s="25" t="n"/>
       <c r="I16" s="25" t="n"/>
     </row>
-    <row r="17" ht="18" customHeight="1" s="62">
+    <row r="17" ht="18" customHeight="1" s="60">
       <c r="A17" s="18" t="n"/>
       <c r="B17" s="23" t="inlineStr">
         <is>
@@ -1583,10 +1583,10 @@
       <c r="C17" s="8" t="n"/>
       <c r="D17" s="25" t="n"/>
       <c r="E17" s="24" t="n"/>
-      <c r="F17" s="71" t="n"/>
-      <c r="I17" s="71" t="n"/>
-    </row>
-    <row r="18" ht="4.5" customHeight="1" s="62">
+      <c r="F17" s="64" t="n"/>
+      <c r="I17" s="64" t="n"/>
+    </row>
+    <row r="18" ht="4.5" customHeight="1" s="60">
       <c r="A18" s="18" t="n"/>
       <c r="B18" s="18" t="n"/>
       <c r="C18" s="8" t="n"/>
@@ -1597,78 +1597,102 @@
       <c r="H18" s="2" t="n"/>
       <c r="I18" s="2" t="n"/>
     </row>
-    <row r="19" ht="18" customHeight="1" s="62">
+    <row r="19" ht="18" customHeight="1" s="60">
       <c r="A19" s="18" t="n"/>
       <c r="B19" s="18" t="n"/>
       <c r="C19" s="8" t="n"/>
-      <c r="D19" s="74" t="inlineStr">
+      <c r="D19" s="67" t="inlineStr">
         <is>
           <t>DESCRIPTION</t>
         </is>
       </c>
-      <c r="E19" s="75" t="n"/>
-      <c r="F19" s="74" t="inlineStr">
+      <c r="E19" s="68" t="n"/>
+      <c r="F19" s="67" t="inlineStr">
         <is>
           <t>QTY</t>
         </is>
       </c>
-      <c r="G19" s="74" t="inlineStr">
+      <c r="G19" s="67" t="inlineStr">
         <is>
           <t>UNIT PRICE</t>
         </is>
       </c>
-      <c r="H19" s="74" t="inlineStr">
+      <c r="H19" s="67" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
       <c r="I19" s="14" t="n"/>
     </row>
-    <row r="20" ht="18" customHeight="1" s="62">
+    <row r="20" ht="18" customHeight="1" s="60">
       <c r="A20" s="18" t="n"/>
       <c r="B20" s="18" t="n"/>
       <c r="C20" s="8" t="n"/>
-      <c r="D20" s="72" t="n"/>
-      <c r="E20" s="73" t="n"/>
-      <c r="F20" s="26" t="n"/>
-      <c r="G20" s="27" t="n"/>
+      <c r="D20" s="65" t="inlineStr">
+        <is>
+          <t>Alendronate Sodium</t>
+        </is>
+      </c>
+      <c r="E20" s="66" t="n"/>
+      <c r="F20" s="26" t="n">
+        <v>34.99</v>
+      </c>
+      <c r="G20" s="27" t="n">
+        <v>3</v>
+      </c>
       <c r="H20" s="27" t="n">
-        <v>0</v>
+        <v>104.97</v>
       </c>
       <c r="I20" s="28" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="62">
+    <row r="21" ht="18" customHeight="1" s="60">
       <c r="A21" s="18" t="n"/>
       <c r="B21" s="18" t="n"/>
       <c r="C21" s="8" t="n"/>
-      <c r="D21" s="59" t="n"/>
-      <c r="E21" s="60" t="n"/>
-      <c r="F21" s="29" t="n"/>
-      <c r="G21" s="30" t="n"/>
+      <c r="D21" s="62" t="inlineStr">
+        <is>
+          <t>Furosemide</t>
+        </is>
+      </c>
+      <c r="E21" s="63" t="n"/>
+      <c r="F21" s="29" t="n">
+        <v>74.97</v>
+      </c>
+      <c r="G21" s="30" t="n">
+        <v>4</v>
+      </c>
       <c r="H21" s="30" t="n">
-        <v>0</v>
+        <v>299.88</v>
       </c>
       <c r="I21" s="28" t="n"/>
     </row>
-    <row r="22" ht="18" customHeight="1" s="62">
+    <row r="22" ht="18" customHeight="1" s="60">
       <c r="A22" s="18" t="n"/>
       <c r="B22" s="18" t="n"/>
       <c r="C22" s="8" t="n"/>
-      <c r="D22" s="63" t="n"/>
-      <c r="E22" s="60" t="n"/>
-      <c r="F22" s="31" t="n"/>
-      <c r="G22" s="32" t="n"/>
+      <c r="D22" s="69" t="inlineStr">
+        <is>
+          <t>Promethazine HCl</t>
+        </is>
+      </c>
+      <c r="E22" s="63" t="n"/>
+      <c r="F22" s="31" t="n">
+        <v>69.93000000000001</v>
+      </c>
+      <c r="G22" s="32" t="n">
+        <v>5</v>
+      </c>
       <c r="H22" s="32" t="n">
-        <v>0</v>
+        <v>349.65</v>
       </c>
       <c r="I22" s="28" t="n"/>
     </row>
-    <row r="23" ht="18" customHeight="1" s="62">
+    <row r="23" ht="18" customHeight="1" s="60">
       <c r="A23" s="18" t="n"/>
       <c r="B23" s="18" t="n"/>
       <c r="C23" s="8" t="n"/>
-      <c r="D23" s="59" t="n"/>
-      <c r="E23" s="60" t="n"/>
+      <c r="D23" s="62" t="n"/>
+      <c r="E23" s="63" t="n"/>
       <c r="F23" s="29" t="n"/>
       <c r="G23" s="30" t="n"/>
       <c r="H23" s="30" t="n">
@@ -1676,12 +1700,12 @@
       </c>
       <c r="I23" s="28" t="n"/>
     </row>
-    <row r="24" ht="18" customHeight="1" s="62">
+    <row r="24" ht="18" customHeight="1" s="60">
       <c r="A24" s="18" t="n"/>
       <c r="B24" s="18" t="n"/>
       <c r="C24" s="8" t="n"/>
-      <c r="D24" s="63" t="n"/>
-      <c r="E24" s="60" t="n"/>
+      <c r="D24" s="69" t="n"/>
+      <c r="E24" s="63" t="n"/>
       <c r="F24" s="31" t="n"/>
       <c r="G24" s="32" t="n"/>
       <c r="H24" s="32" t="n">
@@ -1689,12 +1713,12 @@
       </c>
       <c r="I24" s="28" t="n"/>
     </row>
-    <row r="25" ht="18" customHeight="1" s="62">
+    <row r="25" ht="18" customHeight="1" s="60">
       <c r="A25" s="18" t="n"/>
       <c r="B25" s="18" t="n"/>
       <c r="C25" s="8" t="n"/>
-      <c r="D25" s="59" t="n"/>
-      <c r="E25" s="60" t="n"/>
+      <c r="D25" s="62" t="n"/>
+      <c r="E25" s="63" t="n"/>
       <c r="F25" s="29" t="n"/>
       <c r="G25" s="30" t="n"/>
       <c r="H25" s="30" t="n">
@@ -1702,12 +1726,12 @@
       </c>
       <c r="I25" s="28" t="n"/>
     </row>
-    <row r="26" ht="18" customHeight="1" s="62">
+    <row r="26" ht="18" customHeight="1" s="60">
       <c r="A26" s="18" t="n"/>
       <c r="B26" s="18" t="n"/>
       <c r="C26" s="8" t="n"/>
-      <c r="D26" s="63" t="n"/>
-      <c r="E26" s="60" t="n"/>
+      <c r="D26" s="69" t="n"/>
+      <c r="E26" s="63" t="n"/>
       <c r="F26" s="31" t="n"/>
       <c r="G26" s="32" t="n"/>
       <c r="H26" s="32" t="n">
@@ -1715,12 +1739,12 @@
       </c>
       <c r="I26" s="28" t="n"/>
     </row>
-    <row r="27" ht="18" customHeight="1" s="62">
+    <row r="27" ht="18" customHeight="1" s="60">
       <c r="A27" s="18" t="n"/>
       <c r="B27" s="18" t="n"/>
       <c r="C27" s="8" t="n"/>
-      <c r="D27" s="59" t="n"/>
-      <c r="E27" s="60" t="n"/>
+      <c r="D27" s="62" t="n"/>
+      <c r="E27" s="63" t="n"/>
       <c r="F27" s="29" t="n"/>
       <c r="G27" s="30" t="n"/>
       <c r="H27" s="30" t="n">
@@ -1728,12 +1752,12 @@
       </c>
       <c r="I27" s="28" t="n"/>
     </row>
-    <row r="28" ht="18" customHeight="1" s="62">
+    <row r="28" ht="18" customHeight="1" s="60">
       <c r="A28" s="18" t="n"/>
       <c r="B28" s="18" t="n"/>
       <c r="C28" s="8" t="n"/>
-      <c r="D28" s="63" t="n"/>
-      <c r="E28" s="60" t="n"/>
+      <c r="D28" s="69" t="n"/>
+      <c r="E28" s="63" t="n"/>
       <c r="F28" s="31" t="n"/>
       <c r="G28" s="32" t="n"/>
       <c r="H28" s="32" t="n">
@@ -1741,7 +1765,7 @@
       </c>
       <c r="I28" s="28" t="n"/>
     </row>
-    <row r="29" ht="19.5" customHeight="1" s="62">
+    <row r="29" ht="19.5" customHeight="1" s="60">
       <c r="A29" s="18" t="n"/>
       <c r="B29" s="18" t="n"/>
       <c r="C29" s="8" t="n"/>
@@ -1754,15 +1778,15 @@
         </is>
       </c>
       <c r="H29" s="35" t="n">
-        <v>0</v>
+        <v>754.5</v>
       </c>
       <c r="I29" s="36" t="n"/>
     </row>
-    <row r="30" ht="19.5" customHeight="1" s="62">
+    <row r="30" ht="19.5" customHeight="1" s="60">
       <c r="A30" s="18" t="n"/>
       <c r="B30" s="18" t="n"/>
       <c r="C30" s="8" t="n"/>
-      <c r="D30" s="61" t="inlineStr">
+      <c r="D30" s="70" t="inlineStr">
         <is>
           <t>Remarks / Payment Instructions:</t>
         </is>
@@ -1778,7 +1802,7 @@
       </c>
       <c r="I30" s="36" t="n"/>
     </row>
-    <row r="31" ht="19.5" customHeight="1" s="62">
+    <row r="31" ht="19.5" customHeight="1" s="60">
       <c r="A31" s="18" t="n"/>
       <c r="B31" s="18" t="n"/>
       <c r="C31" s="8" t="n"/>
@@ -1793,7 +1817,7 @@
       </c>
       <c r="I31" s="36" t="n"/>
     </row>
-    <row r="32" ht="19.5" customHeight="1" s="62">
+    <row r="32" ht="19.5" customHeight="1" s="60">
       <c r="A32" s="18" t="n"/>
       <c r="B32" s="18" t="n"/>
       <c r="C32" s="8" t="n"/>
@@ -1808,12 +1832,12 @@
       </c>
       <c r="I32" s="39" t="n"/>
     </row>
-    <row r="33" ht="19.5" customHeight="1" s="62">
+    <row r="33" ht="19.5" customHeight="1" s="60">
       <c r="A33" s="18" t="n"/>
       <c r="B33" s="18" t="n"/>
       <c r="C33" s="8" t="n"/>
-      <c r="D33" s="61" t="n"/>
-      <c r="E33" s="61" t="n"/>
+      <c r="D33" s="70" t="n"/>
+      <c r="E33" s="70" t="n"/>
       <c r="F33" s="34" t="n"/>
       <c r="G33" s="37" t="inlineStr">
         <is>
@@ -1825,12 +1849,12 @@
       </c>
       <c r="I33" s="36" t="n"/>
     </row>
-    <row r="34" ht="19.5" customHeight="1" s="62">
+    <row r="34" ht="19.5" customHeight="1" s="60">
       <c r="A34" s="18" t="n"/>
       <c r="B34" s="18" t="n"/>
       <c r="C34" s="8" t="n"/>
-      <c r="D34" s="61" t="n"/>
-      <c r="E34" s="61" t="n"/>
+      <c r="D34" s="70" t="n"/>
+      <c r="E34" s="70" t="n"/>
       <c r="F34" s="34" t="n"/>
       <c r="G34" s="37" t="inlineStr">
         <is>
@@ -1842,7 +1866,7 @@
       </c>
       <c r="I34" s="41" t="n"/>
     </row>
-    <row r="35" ht="33.75" customHeight="1" s="62">
+    <row r="35" ht="33.75" customHeight="1" s="60">
       <c r="A35" s="18" t="n"/>
       <c r="B35" s="18" t="n"/>
       <c r="C35" s="8" t="n"/>
@@ -1855,51 +1879,51 @@
         </is>
       </c>
       <c r="H35" s="44" t="n">
-        <v>235.66</v>
+        <v>754.5</v>
       </c>
       <c r="I35" s="45" t="n"/>
     </row>
-    <row r="36" ht="9.75" customHeight="1" s="62">
+    <row r="36" ht="9.75" customHeight="1" s="60">
       <c r="A36" s="18" t="n"/>
       <c r="B36" s="18" t="n"/>
       <c r="C36" s="8" t="n"/>
-      <c r="D36" s="68" t="n"/>
-      <c r="I36" s="68" t="n"/>
-    </row>
-    <row r="37" ht="9.75" customHeight="1" s="62">
+      <c r="D36" s="75" t="n"/>
+      <c r="I36" s="75" t="n"/>
+    </row>
+    <row r="37" ht="9.75" customHeight="1" s="60">
       <c r="A37" s="18" t="n"/>
       <c r="B37" s="18" t="n"/>
       <c r="C37" s="8" t="n"/>
-      <c r="D37" s="61" t="n"/>
-      <c r="E37" s="61" t="n"/>
-      <c r="F37" s="68" t="n"/>
-      <c r="G37" s="68" t="n"/>
-      <c r="H37" s="68" t="n"/>
-      <c r="I37" s="68" t="n"/>
-    </row>
-    <row r="38" ht="15.75" customHeight="1" s="62">
+      <c r="D37" s="70" t="n"/>
+      <c r="E37" s="70" t="n"/>
+      <c r="F37" s="75" t="n"/>
+      <c r="G37" s="75" t="n"/>
+      <c r="H37" s="75" t="n"/>
+      <c r="I37" s="75" t="n"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" s="60">
       <c r="A38" s="18" t="n"/>
       <c r="B38" s="18" t="n"/>
       <c r="C38" s="8" t="n"/>
-      <c r="D38" s="61" t="n"/>
-      <c r="E38" s="61" t="n"/>
+      <c r="D38" s="70" t="n"/>
+      <c r="E38" s="70" t="n"/>
       <c r="F38" s="46" t="n"/>
       <c r="G38" s="46" t="n"/>
       <c r="H38" s="46" t="n"/>
       <c r="I38" s="46" t="n"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1" s="62">
+    <row r="39" ht="15.75" customHeight="1" s="60">
       <c r="A39" s="18" t="n"/>
       <c r="B39" s="18" t="n"/>
       <c r="C39" s="8" t="n"/>
-      <c r="D39" s="61" t="n"/>
-      <c r="E39" s="61" t="n"/>
+      <c r="D39" s="70" t="n"/>
+      <c r="E39" s="70" t="n"/>
       <c r="F39" s="47" t="n"/>
       <c r="G39" s="47" t="n"/>
       <c r="H39" s="47" t="n"/>
       <c r="I39" s="47" t="n"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1" s="62">
+    <row r="40" ht="15.75" customHeight="1" s="60">
       <c r="A40" s="18" t="n"/>
       <c r="B40" s="18" t="n"/>
       <c r="C40" s="8" t="n"/>
@@ -1909,23 +1933,23 @@
         </is>
       </c>
       <c r="E40" s="49" t="n"/>
-      <c r="F40" s="66" t="inlineStr">
+      <c r="F40" s="73" t="inlineStr">
         <is>
           <t>Client Signature</t>
         </is>
       </c>
-      <c r="G40" s="67" t="n"/>
+      <c r="G40" s="74" t="n"/>
       <c r="H40" s="47" t="n"/>
       <c r="I40" s="47" t="n"/>
     </row>
-    <row r="41" ht="21" customHeight="1" s="62">
+    <row r="41" ht="21" customHeight="1" s="60">
       <c r="A41" s="50" t="n"/>
       <c r="B41" s="50" t="n"/>
       <c r="C41" s="51" t="n"/>
-      <c r="D41" s="65" t="n"/>
-      <c r="I41" s="65" t="n"/>
-    </row>
-    <row r="42" ht="15.75" customHeight="1" s="62">
+      <c r="D41" s="72" t="n"/>
+      <c r="I41" s="72" t="n"/>
+    </row>
+    <row r="42" ht="15.75" customHeight="1" s="60">
       <c r="A42" s="18" t="n"/>
       <c r="B42" s="18" t="n"/>
       <c r="C42" s="8" t="n"/>
@@ -1936,11 +1960,11 @@
       <c r="H42" s="8" t="n"/>
       <c r="I42" s="8" t="n"/>
     </row>
-    <row r="43" ht="15.75" customHeight="1" s="62">
+    <row r="43" ht="15.75" customHeight="1" s="60">
       <c r="A43" s="18" t="n"/>
       <c r="B43" s="18" t="n"/>
       <c r="C43" s="8" t="n"/>
-      <c r="D43" s="64" t="inlineStr">
+      <c r="D43" s="71" t="inlineStr">
         <is>
           <t>Thank you for your patronage!</t>
         </is>
@@ -1949,14 +1973,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D22:E22"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D30:E32"/>
     <mergeCell ref="D24:E24"/>
@@ -1967,6 +1983,14 @@
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D36:H36"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D22:E22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0" footer="0"/>

</xml_diff>